<commit_message>
TOTAL EXCEL WRITE function update (w/o OVERWRITE)
</commit_message>
<xml_diff>
--- a/data/input_mail/mail_copy_in_format.xlsx
+++ b/data/input_mail/mail_copy_in_format.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="27750" windowHeight="11770" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="27750" windowHeight="11770" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ELMONGY" sheetId="1" r:id="rId1"/>
     <sheet name="YOUSEF" sheetId="2" r:id="rId2"/>
     <sheet name="YOUSEF_MUL" sheetId="10" r:id="rId3"/>
     <sheet name="ELFEKY_MUL" sheetId="3" r:id="rId4"/>
-    <sheet name="AHMED_MUL" sheetId="4" r:id="rId5"/>
+    <sheet name="AHMED_MUL" sheetId="13" r:id="rId5"/>
     <sheet name="SAM" sheetId="9" r:id="rId6"/>
     <sheet name="SAM_MUL" sheetId="5" r:id="rId7"/>
     <sheet name="MIZIOUT" sheetId="6" r:id="rId8"/>
@@ -1272,251 +1272,251 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>AVANTE 2008 KMHDU41BP8U381712</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: DOAA FAYEZ ABD ALLAH ELSAYED ABD ALLAH </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: EMAN ELSAIED MOHY MAKARM </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: AADAWY SAYED AADAWY MOUSTAFA </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2011 KMHDH41DBBU027867</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: MAHMOUD MOHAMED ABD ELAAZIEM ABD ALLAH </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2011 KMHDG41DBBU057026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: NAYROUZ ELSAYED MAMDOUH ELSAYED AHMED HASSANIEN </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2012 KMHDH41DBCU299247</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: GOUNIOR GERGES ESHAQ NASSIEF AWAD </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIVOLI 2015 KPBXHAR1FP019286</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: MAHMOUD MAHMOUD HAGAG TOUNY MOHAMED </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2008 KMHDU41BP8U425062</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUILDING NAME: ELBAHSAMOUN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: REHAM AHMED MOUKHTAR MOHAMED ABD ELKAREEM </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2012 KMHDH41DBCU413802</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: NERMEEN FAWZY MOHAMED LOTFY ABD ELHAMIED </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2011 KMHDH41DBBU034065</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: MAHMOUD ELSAYED YOUNIES SALEM </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2010 KMHDU41BBAU045284</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: AHMED FATHY FAYEZ ELSAYED MOUSTAFA </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K3 2015 KNAFK412BFA326344</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: SALAH SALAMAH MOHAMED ELSAYED ALI YOUSSEF </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2012 KMHDH41DBCU401649</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: NABIELA MOHAMED MOHAMED EBRAHIM </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2012 KMHDH41DBCU617457</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: MOHAMED MOHAMED MORSY ELSHAZLY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2012 KMHDG41DBCU272606</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: ABD ELHAY ABD ELRAZEK QENAWY KAFAFY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TUCSON 2019 KMHJ3812GKU815210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: ROUDINA NASSER MAHROUS AMOUBARK ESMAIL </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FORTE 2011 KNAFU415BBA933829</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: KAREEM HEMDAN GHARABAWY OMAR ELGHARABAWY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2010 KMHDU41BBAU907475</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: ADEL YOUSSEF MOHAMED TOURKY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2011 KMHDG41DBBU024372</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: AHMED MOHAMED ELAAWADY ABD ELAAL </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K3 2013 KNAFZ412BDA004986</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: WALAA GAMIEL FATHY SEDIEK </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2007 KMHDU41BP7U121931</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: ODAY MOHAMED ABD ELAATY MOHAMED MEKAWY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2010 KMHDU41BBAU074145</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: MOSALAM AHMED MAHMOUD ABD ALLAH EBRAHIM </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FORTE 2013 KNAFT415BDA685980</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: HASSAN ELSAYED SABER ABD ELFATAH MOHAMED </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2012 KMHDH41DBCU275493</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: ASHRAF MOHAMED EBRAHIM NASSER </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIVOLI 2018 KPBXH3AR1JP231026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: RAWDA MOAHMED AAFIFY ELSAYED AAFIFY SALAMAH </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FORTE 2009 KNAFH22139A064294</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: KHALED BAHGAT ABD ELGABER AMIEN </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2011 KMHDG41DBBU166305</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: EYAD ALAA SALEH ELSAYED METWALLY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2007 KMHDU41BP7U248439</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: HASSAN SOLIMAN HASSAAN KHEDR </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2010 KMHDU41BBAU005624</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: MAGDA AABOUD HAMAAD BAKRY </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2011 KMHDG41DBBU057458</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSIGNEE NAME: ASMAA FATHY ADREES ABD ELMONAEM MOHAMED </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TUCSON 2020 KMHJ5812GLU324020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVANTE 2007 KMHDU41BP7U018874</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">CONSIGNEE NAME: SHAABAN ELDESSOUKY MOHAMED WAHBA </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2007 KMHDU41BP7U018874</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2008 KMHDU41BP8U381712</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: DOAA FAYEZ ABD ALLAH ELSAYED ABD ALLAH </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: EMAN ELSAIED MOHY MAKARM </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: AADAWY SAYED AADAWY MOUSTAFA </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2011 KMHDH41DBBU027867</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: MAHMOUD MOHAMED ABD ELAAZIEM ABD ALLAH </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2011 KMHDG41DBBU057026</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: NAYROUZ ELSAYED MAMDOUH ELSAYED AHMED HASSANIEN </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2012 KMHDH41DBCU299247</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: GOUNIOR GERGES ESHAQ NASSIEF AWAD </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TIVOLI 2015 KPBXHAR1FP019286</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: MAHMOUD MAHMOUD HAGAG TOUNY MOHAMED </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2008 KMHDU41BP8U425062</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUILDING NAME: ELBAHSAMOUN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: REHAM AHMED MOUKHTAR MOHAMED ABD ELKAREEM </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2012 KMHDH41DBCU413802</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: NERMEEN FAWZY MOHAMED LOTFY ABD ELHAMIED </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2011 KMHDH41DBBU034065</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: MAHMOUD ELSAYED YOUNIES SALEM </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2010 KMHDU41BBAU045284</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: AHMED FATHY FAYEZ ELSAYED MOUSTAFA </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>K3 2015 KNAFK412BFA326344</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: SALAH SALAMAH MOHAMED ELSAYED ALI YOUSSEF </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2012 KMHDH41DBCU401649</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: NABIELA MOHAMED MOHAMED EBRAHIM </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2012 KMHDH41DBCU617457</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: MOHAMED MOHAMED MORSY ELSHAZLY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2012 KMHDG41DBCU272606</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: ABD ELHAY ABD ELRAZEK QENAWY KAFAFY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TUCSON 2019 KMHJ3812GKU815210</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: ROUDINA NASSER MAHROUS AMOUBARK ESMAIL </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FORTE 2011 KNAFU415BBA933829</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: KAREEM HEMDAN GHARABAWY OMAR ELGHARABAWY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2010 KMHDU41BBAU907475</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: ADEL YOUSSEF MOHAMED TOURKY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2011 KMHDG41DBBU024372</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: AHMED MOHAMED ELAAWADY ABD ELAAL </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>K3 2013 KNAFZ412BDA004986</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: WALAA GAMIEL FATHY SEDIEK </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2007 KMHDU41BP7U121931</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: ODAY MOHAMED ABD ELAATY MOHAMED MEKAWY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2010 KMHDU41BBAU074145</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: MOSALAM AHMED MAHMOUD ABD ALLAH EBRAHIM </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FORTE 2013 KNAFT415BDA685980</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: HASSAN ELSAYED SABER ABD ELFATAH MOHAMED </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2012 KMHDH41DBCU275493</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: ASHRAF MOHAMED EBRAHIM NASSER </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TIVOLI 2018 KPBXH3AR1JP231026</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: RAWDA MOAHMED AAFIFY ELSAYED AAFIFY SALAMAH </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FORTE 2009 KNAFH22139A064294</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: KHALED BAHGAT ABD ELGABER AMIEN </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2011 KMHDG41DBBU166305</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: EYAD ALAA SALEH ELSAYED METWALLY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2007 KMHDU41BP7U248439</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: HASSAN SOLIMAN HASSAAN KHEDR </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2010 KMHDU41BBAU005624</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: MAGDA AABOUD HAMAAD BAKRY </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVANTE 2011 KMHDG41DBBU057458</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSIGNEE NAME: ASMAA FATHY ADREES ABD ELMONAEM MOHAMED </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TUCSON 2020 KMHJ5812GLU324020</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
@@ -2256,7 +2256,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
@@ -2316,12 +2316,12 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.45">
@@ -2381,12 +2381,12 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
@@ -2446,12 +2446,12 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
@@ -2511,12 +2511,12 @@
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.45">
@@ -2576,12 +2576,12 @@
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.45">
@@ -2641,17 +2641,17 @@
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.45">
@@ -2706,12 +2706,12 @@
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.45">
@@ -2771,12 +2771,12 @@
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.45">
@@ -2836,12 +2836,12 @@
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.45">
@@ -2901,12 +2901,12 @@
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.45">
@@ -2966,12 +2966,12 @@
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.45">
@@ -3031,12 +3031,12 @@
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.45">
@@ -3096,12 +3096,12 @@
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.45">
@@ -3161,12 +3161,12 @@
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.45">
@@ -3226,12 +3226,12 @@
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.45">
@@ -3291,12 +3291,12 @@
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.45">
@@ -3365,8 +3365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3753,14 +3753,14 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>408</v>
+        <v>467</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>407</v>
+        <v>468</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.45">
@@ -3829,8 +3829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4442,8 +4442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4688,8 +4688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -5614,7 +5614,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5622,8 +5621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A194"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="H151" sqref="H151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -5658,12 +5657,12 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
@@ -5723,12 +5722,12 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
@@ -5788,12 +5787,12 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
@@ -5853,12 +5852,12 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
@@ -5918,12 +5917,12 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
@@ -5983,12 +5982,12 @@
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.45">
@@ -6048,12 +6047,12 @@
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.45">
@@ -6113,12 +6112,12 @@
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.45">
@@ -6178,12 +6177,12 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.45">
@@ -6238,12 +6237,12 @@
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.45">
@@ -6303,12 +6302,12 @@
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.45">
@@ -6368,12 +6367,12 @@
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.45">
@@ -6437,8 +6436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -6691,7 +6690,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>

</xml_diff>

<commit_message>
EDI/H_BL_NO generation algorithm update ver
</commit_message>
<xml_diff>
--- a/data/input_mail/mail_copy_in_format.xlsx
+++ b/data/input_mail/mail_copy_in_format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="27750" windowHeight="11770" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="27750" windowHeight="11770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ELMONGY" sheetId="1" r:id="rId1"/>
@@ -3365,8 +3365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="L82" sqref="L82"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4688,8 +4688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127:A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -5621,7 +5621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A194"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
+    <sheetView topLeftCell="A156" workbookViewId="0">
       <selection activeCell="H151" sqref="H151"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
release initial MACRO format sheet feature ver
</commit_message>
<xml_diff>
--- a/data/input_mail/mail_copy_in_format.xlsx
+++ b/data/input_mail/mail_copy_in_format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="27750" windowHeight="11770" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="27750" windowHeight="11770" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ELMONGY" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="EGY_KOREA" sheetId="7" r:id="rId9"/>
     <sheet name="AL_AMAL" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1059,9 +1059,6 @@
     <t>ACID NO: 9992022070000032918</t>
   </si>
   <si>
-    <t>ACID NO: 9992022070000034542</t>
-  </si>
-  <si>
     <t>ACID NO: 9992022070000042040</t>
   </si>
   <si>
@@ -1312,10 +1309,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TIVOLI 2015 KPBXHAR1FP019286</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">CONSIGNEE NAME: MAHMOUD MAHMOUD HAGAG TOUNY MOHAMED </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1517,6 +1510,14 @@
   </si>
   <si>
     <t xml:space="preserve">CONSIGNEE NAME: SHAABAN ELDESSOUKY MOHAMED WAHBA </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIVOLI 2015 KPBXH3AR1FP019286</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACID NO: 999202070000034542</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2148,8 +2149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A292"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="E86" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2186,12 +2187,12 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
@@ -2251,12 +2252,12 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
@@ -2316,12 +2317,12 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.45">
@@ -2381,12 +2382,12 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
@@ -2446,12 +2447,12 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
@@ -2511,12 +2512,12 @@
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.45">
@@ -2576,12 +2577,12 @@
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>417</v>
+        <v>467</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.45">
@@ -2616,7 +2617,7 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>337</v>
+        <v>468</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.45">
@@ -2641,17 +2642,17 @@
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.45">
@@ -2681,7 +2682,7 @@
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.45">
@@ -2706,12 +2707,12 @@
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.45">
@@ -2746,7 +2747,7 @@
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.45">
@@ -2756,7 +2757,7 @@
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.45">
@@ -2771,12 +2772,12 @@
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.45">
@@ -2811,7 +2812,7 @@
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.45">
@@ -2821,7 +2822,7 @@
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.45">
@@ -2836,12 +2837,12 @@
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.45">
@@ -2876,7 +2877,7 @@
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.45">
@@ -2886,7 +2887,7 @@
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.45">
@@ -2901,12 +2902,12 @@
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.45">
@@ -2941,7 +2942,7 @@
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.45">
@@ -2951,7 +2952,7 @@
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.45">
@@ -2966,12 +2967,12 @@
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.45">
@@ -3006,7 +3007,7 @@
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.45">
@@ -3016,7 +3017,7 @@
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.45">
@@ -3031,12 +3032,12 @@
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.45">
@@ -3071,7 +3072,7 @@
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.45">
@@ -3081,7 +3082,7 @@
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.45">
@@ -3096,12 +3097,12 @@
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.45">
@@ -3136,7 +3137,7 @@
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.45">
@@ -3146,7 +3147,7 @@
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.45">
@@ -3161,12 +3162,12 @@
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.45">
@@ -3196,12 +3197,12 @@
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.45">
@@ -3226,12 +3227,12 @@
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.45">
@@ -3261,12 +3262,12 @@
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.45">
@@ -3291,12 +3292,12 @@
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.45">
@@ -3326,12 +3327,12 @@
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.45">
@@ -3365,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:A102"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3753,29 +3754,29 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.45">
@@ -3785,17 +3786,17 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.45">
@@ -3805,7 +3806,7 @@
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.45">
@@ -5657,22 +5658,22 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
@@ -5687,17 +5688,17 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
@@ -5707,7 +5708,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
@@ -5722,22 +5723,22 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
@@ -5752,17 +5753,17 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
@@ -5772,7 +5773,7 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.45">
@@ -5787,22 +5788,22 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.45">
@@ -5817,17 +5818,17 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.45">
@@ -5837,7 +5838,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.45">
@@ -5852,22 +5853,22 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.45">
@@ -5882,17 +5883,17 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.45">
@@ -5902,7 +5903,7 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.45">
@@ -5917,17 +5918,17 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
@@ -5947,17 +5948,17 @@
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.45">
@@ -5967,7 +5968,7 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.45">
@@ -5982,22 +5983,22 @@
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.45">
@@ -6012,17 +6013,17 @@
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.45">
@@ -6032,7 +6033,7 @@
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.45">
@@ -6047,27 +6048,27 @@
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.45">
@@ -6077,17 +6078,17 @@
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.45">
@@ -6097,7 +6098,7 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.45">
@@ -6112,22 +6113,22 @@
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.45">
@@ -6142,17 +6143,17 @@
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.45">
@@ -6162,7 +6163,7 @@
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.45">
@@ -6177,17 +6178,17 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.45">
@@ -6202,17 +6203,17 @@
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.45">
@@ -6237,22 +6238,22 @@
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.45">
@@ -6267,17 +6268,17 @@
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.45">
@@ -6302,17 +6303,17 @@
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.45">
@@ -6332,17 +6333,17 @@
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.45">
@@ -6367,17 +6368,17 @@
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.45">
@@ -6392,17 +6393,17 @@
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.45">
@@ -6690,7 +6691,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -6811,7 +6812,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">

</xml_diff>